<commit_message>
Listagem inicial dos requisitos
</commit_message>
<xml_diff>
--- a/PastaDocsRequisitos/2SIR-ListaPesquisa.xlsx
+++ b/PastaDocsRequisitos/2SIR-ListaPesquisa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alice\OneDrive\Área de Trabalho\Arquivos Faculdade\Segundo ano\Engenharia de software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A2DC5E-72AB-4D94-9499-0C0CB49D6B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E1C79B-201C-4CB8-9FFA-7BC949A1F9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0891ED88-779E-4904-AB47-DA324D9A5ACC}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Requisitos do sistema de gestão de estacionamento</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>.Cadastramento e tipificaçao de vaga</t>
-  </si>
-  <si>
-    <t>.Integraçao com sistema da policia para verificar possivel roubo</t>
   </si>
 </sst>
 </file>
@@ -473,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CD8592-6EB6-4B54-8F7E-C6467C02028C}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,11 +616,6 @@
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>